<commit_message>
javascript files for everyone
</commit_message>
<xml_diff>
--- a/Example for Login and Design/excel/default_solar.xlsx
+++ b/Example for Login and Design/excel/default_solar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/PHPExcel-develop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Airkick/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -862,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -990,10 +990,10 @@
         <v>82</v>
       </c>
       <c r="D28">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
validation for numbers on excel sheets
</commit_message>
<xml_diff>
--- a/Example for Login and Design/excel/default_solar.xlsx
+++ b/Example for Login and Design/excel/default_solar.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="920" windowWidth="15420" windowHeight="15220" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="400" yWindow="920" windowWidth="15420" windowHeight="15220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Indata och resultat privatperso" sheetId="1" r:id="rId1"/>
@@ -853,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1560,6 +1560,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18 B20 B24 B28 B32 B33 B35 B36 B37 B38 B53 B60 B61 B62 B63 B64 B65 B66 B67 B68 B65">
+      <formula1>-100000</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1568,8 +1573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2275,6 +2280,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18 B20 B24 B28 B32 B33 B35 B36 B37 B38 B53 B60 B61 B62 B63 B64 B65 B66 B67 B68 B33 B38 B35 B53 B60 B61 B68 B66 B65 B64 B63">
+      <formula1>-100000</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2283,8 +2293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2925,6 +2935,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 B16 B17 B18 B20 B21 B23 B24 B30 B31 B50 B51 B56 B60 B64 B65 B66 B51 B56 B51 B31 B30 B24 B21">
+      <formula1>-100000</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2933,8 +2948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3575,6 +3590,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 B16 B18 B20 B21 B23 B24 B30 B31 B32 B33 B34 B35 B36 B37 B41 B42 B43 B44 B45 B50 B51 B56 B60 B64 B65 B66 B64">
+      <formula1>-1000000</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>